<commit_message>
Nearly finished settings & Added excel file implementation
</commit_message>
<xml_diff>
--- a/valorant.xlsx
+++ b/valorant.xlsx
@@ -217,7 +217,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,7 +363,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,7 +421,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
         <v>16</v>
       </c>
@@ -468,7 +468,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -515,7 +515,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>26</v>
       </c>
@@ -562,13 +562,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://tracker.gg/valorant/match/af835a6e-2154-4344-a96c-662a3189fc8f"/>
-    <hyperlink ref="H2" r:id="rId2" display="https://youtu.be/_m9aXob8GEA"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Finished excel implementation, Removed spreadsheet_to_read  & Changed SPREADSHEET_FORMAT_OPTIONS in constants.py slightly
</commit_message>
<xml_diff>
--- a/valorant.xlsx
+++ b/valorant.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -68,63 +68,17 @@
   </si>
   <si>
     <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ff47c7f1-4b83-426a-b091-d79f940bd3c2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Diamond 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://tracker.gg/valorant/match/af835a6e-2154-4344-a96c-662a3189fc8f</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://youtu.be/_m9aXob8GEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lotus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Viper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://tracker.gg/valorant/match/ff47c7f1-4b83-426a-b091-d79f940bd3c2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://youtu.be/kn0jEd5tJkk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sunset</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Omen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ef7dc8e6-03a3-40bc-a16a-9f28a571c72d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://tracker.gg/valorant/match/ef7dc8e6-03a3-40bc-a16a-9f28a571c72d</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://youtu.be/cF3BohIa63A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bind</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brimstone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -145,19 +99,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -208,7 +149,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -218,22 +159,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -363,7 +288,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -421,149 +346,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>45390</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="5" t="n">
-        <v>-15</v>
-      </c>
-      <c r="E2" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="F2" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="L2" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="M2" s="5" t="n">
-        <v>6</v>
-      </c>
-      <c r="N2" s="5" t="n">
-        <v>24</v>
-      </c>
-      <c r="O2" s="5" t="n">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>45390</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="5" t="n">
-        <v>-12</v>
-      </c>
-      <c r="E3" s="5" t="n">
-        <v>11</v>
-      </c>
-      <c r="F3" s="5" t="n">
-        <v>13</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="K3" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="L3" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="M3" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="N3" s="5" t="n">
-        <v>40</v>
-      </c>
-      <c r="O3" s="5" t="n">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="90.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="4" t="n">
-        <v>45389</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="5" t="n">
-        <v>-11</v>
-      </c>
-      <c r="E4" s="5" t="n">
-        <v>12</v>
-      </c>
-      <c r="F4" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="M4" s="5" t="n">
-        <v>14</v>
-      </c>
-      <c r="N4" s="5" t="n">
-        <v>23</v>
-      </c>
-      <c r="O4" s="5" t="n">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added max_videos_simultaneously and latest_match_id settings & Removed latest_match_id.txt implementation
</commit_message>
<xml_diff>
--- a/valorant.xlsx
+++ b/valorant.xlsx
@@ -288,7 +288,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,6 +345,31 @@
       <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
     </row>
     <row r="1048576" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>

</xml_diff>